<commit_message>
Updated the movie's data reading selectors to the new IMDb view.
</commit_message>
<xml_diff>
--- a/Project4-PersonalUseAutomation/Top Box Office Movies US_BasicVersion/Data/IMDb Top Box Office Movies Data.xlsx
+++ b/Project4-PersonalUseAutomation/Top Box Office Movies US_BasicVersion/Data/IMDb Top Box Office Movies Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MyProjects\UiPath\Project4_PersonalUseAutomation\Top Box Office Movies US_BasicVersion\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MyProjects\UiPath\Udacity\Project4-PersonalUseAutomation\Top Box Office Movies US_BasicVersion\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD39FC2-C985-4EAD-A93C-D851B60C2DD8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5773E3-66A8-4547-9527-103B6A7A2919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="30" windowWidth="20460" windowHeight="11010" xr2:uid="{50049FA4-2F02-45C3-8D33-348569F0BB8A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>Title</t>
   </si>
@@ -60,165 +60,163 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Wrath of Man</t>
-  </si>
-  <si>
-    <t>The plot follows H, a cold and mysterious character working at a cash truck company responsible for moving hundreds of millions of dollars around Los Angeles each week.</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
-    <t>1h 59min</t>
-  </si>
-  <si>
-    <t>Action, 
-Thriller</t>
-  </si>
-  <si>
-    <t>7 May 2021 (USA)</t>
-  </si>
-  <si>
-    <t>Kimetsu no Yaiba: Mugen Ressha-Hen</t>
-  </si>
-  <si>
-    <t>Tanjiro Kamado, joined with Inosuke Hashibira, a boy raised by boars who wears a boar's head, and Zenitsu Agatsuma, a scared boy who reveals his true power when he sleeps, board the Infinity Train on a new mission with the Flame Pillar, Kyojuro Rengoku, to defeat a demon who has been tormenting the people and killing the demon slayers who oppose it!</t>
-  </si>
-  <si>
-    <t>1h 57min</t>
-  </si>
-  <si>
-    <t>Animation, 
-Action, 
-Adventure</t>
-  </si>
-  <si>
-    <t>23 April 2021 (USA)</t>
-  </si>
-  <si>
-    <t>Mortal Kombat</t>
-  </si>
-  <si>
-    <t>MMA fighter Cole Young (Lewis Tan), accustomed to taking a beating for money, is unaware of his heritage-or why Outworld's Emperor Shang Tsung (Chin Han) has sent his best warrior, Sub-Zero (Joe Taslim), an otherworldly Cryomancer, to hunt Cole down. Fearing for his family's safety, Cole goes in search of Sonya Blade (Jessica McNamee) at the direction of Jax (Mehcad Brooks), a Special Forces Major who bears the same strange dragon marking Cole was born with. Soon, he finds himself at the temple of Lord Raiden (Tadanobu Asano), an Elder God and the protector of Earthrealm, who grants sanctuary to those who bear the mark. Here, Cole trains with experienced warriors Liu Kang (Ludi Lin), Kung Lao (Max Huang) and rogue mercenary Kano (Josh Lawson), as he prepares to stand with Earth's greatest champions against the enemies of Outworld in a high stakes battle for the universe. But will Cole be pushed hard enough to unlock his arcana-the immense power from within his soul-in time to save not...
-                Written by
-Warner Bros.</t>
-  </si>
-  <si>
-    <t>1h 50min</t>
-  </si>
-  <si>
-    <t>Action, 
-Adventure, 
-Fantasy</t>
-  </si>
-  <si>
-    <t>Godzilla vs. Kong</t>
-  </si>
-  <si>
-    <t>Legends collide as Godzilla and Kong, the two most powerful forces of nature, clash on the big screen in a spectacular battle for the ages. As a squadron embarks on a perilous mission into fantastic uncharted terrain, unearthing clues to the Titans' very origins and mankind's survival, a conspiracy threatens to wipe the creatures, both good and bad, from the face of the earth forever.
-                Written by
-Warner Bros.</t>
-  </si>
-  <si>
     <t>PG-13</t>
   </si>
   <si>
-    <t>1h 53min</t>
-  </si>
-  <si>
-    <t>Action, 
-Sci-Fi, 
-Thriller</t>
-  </si>
-  <si>
-    <t>31 March 2021 (USA)</t>
-  </si>
-  <si>
-    <t>Raya and the Last Dragon</t>
-  </si>
-  <si>
-    <t>Long ago, in the fantasy world of Kumandra, humans and dragons lived together in harmony. However, when sinister monsters known as the Druun threatened the land, the dragons sacrificed themselves to save humanity. Now, 500 years later, those same monsters have returned, and it's up to a lone warrior to track down the last dragon and stop the Druun for good.</t>
-  </si>
-  <si>
-    <t>PG</t>
-  </si>
-  <si>
     <t>1h 47min</t>
   </si>
   <si>
-    <t>5 March 2021 (USA)</t>
-  </si>
-  <si>
-    <t>Here Today</t>
-  </si>
-  <si>
-    <t>When veteran comedy writer Charlie Burnz meets New York street singer Emma Payge, they form an unlikely yet hilarious and touching friendship that kicks the generation gap aside and redefines the meaning of love and trust.</t>
-  </si>
-  <si>
-    <t>Comedy</t>
-  </si>
-  <si>
-    <t>Spiral: From the Book of Saw</t>
-  </si>
-  <si>
-    <t>Working in the shadow of his father, an esteemed police veteran (Samuel L. Jackson), brash Detective Ezekiel "Zeke" Banks (Chris Rock) and his rookie partner (Max Minghella) take charge of a grisly investigation into murders that are eerily reminiscent of the city's gruesome past. Unwittingly entrapped in a deepening mystery, Zeke finds himself at the center of the killer's morbid game.
-                Written by
-Lionsgate</t>
-  </si>
-  <si>
-    <t>1h 33min</t>
-  </si>
-  <si>
-    <t>Crime, 
-Horror, 
-Mystery</t>
-  </si>
-  <si>
-    <t>14 May 2021 (USA)</t>
-  </si>
-  <si>
-    <t>Those Who Wish Me Dead</t>
-  </si>
-  <si>
-    <t>A teenage murder witness finds himself pursued by twin assassins in the Montana wilderness with a survival expert tasked with protecting him -- and a forest fire threatening to consume them all.</t>
-  </si>
-  <si>
-    <t>1h 40min</t>
-  </si>
-  <si>
-    <t>Action, 
-Drama, 
-Thriller</t>
-  </si>
-  <si>
-    <t>Finding You</t>
-  </si>
-  <si>
-    <t>Finley, a talented aspiring violinist, meets Beckett, a famous young movie star, on the way to her college semester abroad program in a small coastal village in Ireland. An unexpected romance emerges as the heartthrob Beckett leads the uptight Finley on an adventurous reawakening, and she emboldens him to take charge of his future, until the pressures of his stardom get in the way.
-                Written by
-RS</t>
-  </si>
-  <si>
     <t>1h 55min</t>
   </si>
   <si>
-    <t>Drama, 
-Romance</t>
-  </si>
-  <si>
-    <t>Profile</t>
-  </si>
-  <si>
-    <t>A British journalist goes undercover and infiltrates the digital propaganda channels of the so-called Islamic State, which has been mobilizing ever greater numbers of women from Europe. Her daily Internet contacts with an ISIS recruiter gradually pull her in and push the limits of her investigation.
-                Written by
-Markus Fagerholt</t>
-  </si>
-  <si>
-    <t>1h 46min</t>
-  </si>
-  <si>
-    <t>Mystery, 
-Thriller</t>
+    <t>Shang-Chi and the Legend of the Ten Rings</t>
+  </si>
+  <si>
+    <t>Shang-Chi, the master of weaponry-based Kung Fu, is forced to confront his past after being drawn into the Ten Rings organization.</t>
+  </si>
+  <si>
+    <t>97K</t>
+  </si>
+  <si>
+    <t>2h 12min</t>
+  </si>
+  <si>
+    <t>Action,Adventure,Fantasy</t>
+  </si>
+  <si>
+    <t>Dear Evan Hansen</t>
+  </si>
+  <si>
+    <t>Film adaptation of the Tony and Grammy Award-winning musical about Evan Hansen, a high school senior with Social Anxiety disorder and his journey of self-discovery and acceptance following the suicide of a fellow classmate.</t>
+  </si>
+  <si>
+    <t>3.8K</t>
+  </si>
+  <si>
+    <t>2h 17min</t>
+  </si>
+  <si>
+    <t>Drama,Musical</t>
+  </si>
+  <si>
+    <t>Free Guy</t>
+  </si>
+  <si>
+    <t>A bank teller discovers that he's actually an NPC inside a brutal, open world video game.</t>
+  </si>
+  <si>
+    <t>105K</t>
+  </si>
+  <si>
+    <t>Action,Adventure,Comedy</t>
+  </si>
+  <si>
+    <t>Candyman</t>
+  </si>
+  <si>
+    <t>A sequel to the horror film Candyman (1992) that returns to the now-gentrified Chicago neighborhood where the legend began.</t>
+  </si>
+  <si>
+    <t>30K</t>
+  </si>
+  <si>
+    <t>1h 31min</t>
+  </si>
+  <si>
+    <t>Horror,Thriller</t>
+  </si>
+  <si>
+    <t>Cry Macho</t>
+  </si>
+  <si>
+    <t>A one-time rodeo star and washed-up horse breeder takes a job to bring a man's young son home and away from his alcoholic mom. On their journey, the horseman finds redemption through teaching the boy what it means to be a good man.</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>1h 44min</t>
+  </si>
+  <si>
+    <t>Drama,Thriller,Western</t>
+  </si>
+  <si>
+    <t>Jungle Cruise</t>
+  </si>
+  <si>
+    <t>Based on Disneyland's theme park ride where a small riverboat takes a group of travelers through a jungle filled with dangerous animals and reptiles but with a supernatural element.</t>
+  </si>
+  <si>
+    <t>107K</t>
+  </si>
+  <si>
+    <t>2h 7min</t>
+  </si>
+  <si>
+    <t>Malignant</t>
+  </si>
+  <si>
+    <t>Madison is paralyzed by shocking visions of grisly murders, and her torment worsens as she discovers that these waking dreams are in fact terrifying realities.</t>
+  </si>
+  <si>
+    <t>44K</t>
+  </si>
+  <si>
+    <t>1h 51min</t>
+  </si>
+  <si>
+    <t>Crime,Horror,Mystery</t>
+  </si>
+  <si>
+    <t>Copshop</t>
+  </si>
+  <si>
+    <t>On the run from a lethal assassin, a wily con artist devises a scheme to hide out inside a small-town police station-but when the hitman turns up at the precinct, an unsuspecting rookie cop finds herself caught in the crosshairs.</t>
+  </si>
+  <si>
+    <t>2.5K</t>
+  </si>
+  <si>
+    <t>Action,Crime,Thriller</t>
+  </si>
+  <si>
+    <t>PAW Patrol: The Movie</t>
+  </si>
+  <si>
+    <t>Ryder and the pups are called to Adventure City to stop Mayor Humdinger from turning the bustling metropolis into a state of chaos.</t>
+  </si>
+  <si>
+    <t>3.5K</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>1h 26min</t>
+  </si>
+  <si>
+    <t>Animation,Adventure,Comedy</t>
+  </si>
+  <si>
+    <t>Love Story</t>
+  </si>
+  <si>
+    <t>A love story of a boy and girl who move to the city from their village to pursue their dreams.</t>
+  </si>
+  <si>
+    <t>1.4K</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35min </t>
+  </si>
+  <si>
+    <t>Romance</t>
   </si>
 </sst>
 </file>
@@ -606,264 +604,264 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="285" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="C2">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1">
-        <v>4213</v>
+        <v>7.9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" t="s">
-        <v>41</v>
+        <v>16</v>
+      </c>
+      <c r="H2">
+        <v>2021</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>7.4</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="285" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6">
+        <v>5.8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
         <v>9</v>
       </c>
-      <c r="C3">
-        <v>7.4</v>
-      </c>
-      <c r="D3" s="1">
-        <v>7151</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="390" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="F6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="375" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7">
+        <v>6.6</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="330" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8">
+        <v>6.3</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
         <v>43</v>
       </c>
-      <c r="C4">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1">
-        <v>14638</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5">
-        <v>8.5</v>
-      </c>
-      <c r="D5" s="1">
-        <v>18180</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6">
-        <v>7.4</v>
-      </c>
-      <c r="D6" s="1">
-        <v>57961</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7">
-        <v>6.5</v>
-      </c>
-      <c r="D7" s="1">
-        <v>126916</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8">
-        <v>6.2</v>
-      </c>
-      <c r="D8" s="1">
-        <v>97998</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" t="s">
-        <v>18</v>
+      <c r="H8">
+        <v>2021</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9">
+        <v>6.7</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C9">
-        <v>6.5</v>
-      </c>
-      <c r="D9" s="1">
-        <v>209</v>
-      </c>
       <c r="E9" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="255" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>49</v>
       </c>
-      <c r="H9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10">
+        <v>6.2</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C10">
-        <v>7</v>
-      </c>
-      <c r="D10" s="1">
-        <v>606</v>
-      </c>
       <c r="E10" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="F10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H10" t="s">
-        <v>41</v>
+        <v>54</v>
+      </c>
+      <c r="H10">
+        <v>2021</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="C11">
-        <v>6.1</v>
-      </c>
-      <c r="D11" s="1">
-        <v>295</v>
+        <v>8</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
       <c r="F11" t="s">
-        <v>16</v>
+        <v>59</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H11" t="s">
-        <v>13</v>
+        <v>60</v>
+      </c>
+      <c r="H11">
+        <v>2021</v>
       </c>
     </row>
   </sheetData>

</xml_diff>